<commit_message>
Added new funcs for word and phrase frequency,
scrivener file with Abstract
</commit_message>
<xml_diff>
--- a/OronymsPushbacksTemplate.xlsx
+++ b/OronymsPushbacksTemplate.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="18340" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="emptyOurEmailOronymsPushback" sheetId="2" r:id="rId1"/>
-    <sheet name="anicecoldhourOronymsPushback.cs" sheetId="1" r:id="rId2"/>
+    <sheet name="ActualAnswersOronymsPushback" sheetId="3" r:id="rId1"/>
+    <sheet name="emptyOurEmailOronymsPushback" sheetId="2" r:id="rId2"/>
+    <sheet name="anicecoldhourOronymsPushback.cs" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="384">
   <si>
     <t>orthoPhrases.push_back(</t>
   </si>
@@ -920,16 +921,275 @@
   </si>
   <si>
     <t>empty our email ___SUCCESS!___</t>
+  </si>
+  <si>
+    <t>a nice cold hour</t>
+  </si>
+  <si>
+    <t>a nights cold hour</t>
+  </si>
+  <si>
+    <t>an ice cold hour</t>
+  </si>
+  <si>
+    <t>a nice cold dour</t>
+  </si>
+  <si>
+    <t>a nice coal dower</t>
+  </si>
+  <si>
+    <t>a nice cold thou are</t>
+  </si>
+  <si>
+    <t>a nice coal dour</t>
+  </si>
+  <si>
+    <t>a nice old hour</t>
+  </si>
+  <si>
+    <t>a nice hold hour</t>
+  </si>
+  <si>
+    <t>a nice gold hour</t>
+  </si>
+  <si>
+    <t>a nice scored hour</t>
+  </si>
+  <si>
+    <t>a nice scold hour</t>
+  </si>
+  <si>
+    <t>ah nay skull dower</t>
+  </si>
+  <si>
+    <t>a nye scoldower</t>
+  </si>
+  <si>
+    <t>a nice bold hour</t>
+  </si>
+  <si>
+    <t>a nice gold dollar</t>
+  </si>
+  <si>
+    <t>a nice odd hour</t>
+  </si>
+  <si>
+    <t>a nice spoke hour</t>
+  </si>
+  <si>
+    <t>a nice cold our</t>
+  </si>
+  <si>
+    <t>a nice godfather</t>
+  </si>
+  <si>
+    <t>an ice cold our</t>
+  </si>
+  <si>
+    <t>an ice gold hour</t>
+  </si>
+  <si>
+    <t>an ice scold hour</t>
+  </si>
+  <si>
+    <t>an eye scold hour</t>
+  </si>
+  <si>
+    <t>an ice old hour</t>
+  </si>
+  <si>
+    <t>an eye scol dagr</t>
+  </si>
+  <si>
+    <t>an eyes cold hour</t>
+  </si>
+  <si>
+    <t>in ice cold hour</t>
+  </si>
+  <si>
+    <t>an ounce gold hour</t>
+  </si>
+  <si>
+    <t>and i scold our</t>
+  </si>
+  <si>
+    <t>on ice coal dour</t>
+  </si>
+  <si>
+    <t>an i scold hour</t>
+  </si>
+  <si>
+    <t>an iced cold hour</t>
+  </si>
+  <si>
+    <t>in ice cold davar</t>
+  </si>
+  <si>
+    <t>in icecube daver</t>
+  </si>
+  <si>
+    <t>an ice cold bowl</t>
+  </si>
+  <si>
+    <t>i saw tower</t>
+  </si>
+  <si>
+    <t>an ice cold dour</t>
+  </si>
+  <si>
+    <t>an ice coal dower</t>
+  </si>
+  <si>
+    <t>an ice cold dower</t>
+  </si>
+  <si>
+    <t>and ice cold dollar</t>
+  </si>
+  <si>
+    <t>an ice coal dour</t>
+  </si>
+  <si>
+    <t>an ice cold bower</t>
+  </si>
+  <si>
+    <t>a nice cool hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can i score the hour  </t>
+  </si>
+  <si>
+    <t>in ice co daver</t>
+  </si>
+  <si>
+    <t>an icecold hour</t>
+  </si>
+  <si>
+    <t>an ice cold dollar</t>
+  </si>
+  <si>
+    <t>an ice core bower</t>
+  </si>
+  <si>
+    <t>a nice cool bowl</t>
+  </si>
+  <si>
+    <t>an ice cove daver</t>
+  </si>
+  <si>
+    <t>a niceco daver</t>
+  </si>
+  <si>
+    <t>an ice called dower</t>
+  </si>
+  <si>
+    <t>in ice code our</t>
+  </si>
+  <si>
+    <t>in a ice cold hour</t>
+  </si>
+  <si>
+    <t>an ice could hour</t>
+  </si>
+  <si>
+    <t>in unschooled hour</t>
+  </si>
+  <si>
+    <t>in the eyeschool tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the ice cold hour </t>
+  </si>
+  <si>
+    <t>in ice called our</t>
+  </si>
+  <si>
+    <t>in the ice cold hour</t>
+  </si>
+  <si>
+    <t>in ice coal dour</t>
+  </si>
+  <si>
+    <t>in ice cold our</t>
+  </si>
+  <si>
+    <t>a nice cool dollar</t>
+  </si>
+  <si>
+    <t>an ice cold thou are</t>
+  </si>
+  <si>
+    <t>a light cold hour</t>
+  </si>
+  <si>
+    <t>an nice cold hour</t>
+  </si>
+  <si>
+    <t>in nice cold hour</t>
+  </si>
+  <si>
+    <t>on ice col dour</t>
+  </si>
+  <si>
+    <t>on the ice cold hour</t>
+  </si>
+  <si>
+    <t>on ice called our</t>
+  </si>
+  <si>
+    <t>on ice cold hour</t>
+  </si>
+  <si>
+    <t>on ice cold dower</t>
+  </si>
+  <si>
+    <t>on ice cold bauer</t>
+  </si>
+  <si>
+    <t>on the ice cold dour</t>
+  </si>
+  <si>
+    <t>all ice cold hour</t>
+  </si>
+  <si>
+    <t>on ice cold thou art</t>
+  </si>
+  <si>
+    <t>on ice old hour</t>
+  </si>
+  <si>
+    <t>on eis kol dour</t>
+  </si>
+  <si>
+    <t>a nice pollard</t>
+  </si>
+  <si>
+    <t>on a nice cold hour</t>
+  </si>
+  <si>
+    <t>on ice cold air</t>
+  </si>
+  <si>
+    <t>all eyes cold hour</t>
+  </si>
+  <si>
+    <t>on iced cold hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -955,8 +1215,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1290,18 +1554,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:C8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>292</v>
+      <c r="B1" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1311,8 +1579,8 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>293</v>
+      <c r="B2" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1322,8 +1590,8 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>294</v>
+      <c r="B3" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1333,8 +1601,8 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
-        <v>295</v>
+      <c r="B4" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1344,8 +1612,8 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
-        <v>296</v>
+      <c r="B5" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1355,8 +1623,8 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
-        <v>297</v>
+      <c r="B6" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1366,8 +1634,8 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>298</v>
+      <c r="B7" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1377,8 +1645,8 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
-        <v>299</v>
+      <c r="B8" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1388,6 +1656,9 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -1396,6 +1667,9 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
@@ -1404,6 +1678,9 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
@@ -1412,6 +1689,9 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
@@ -1420,6 +1700,9 @@
       <c r="A13" t="s">
         <v>0</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
@@ -1428,6 +1711,9 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
@@ -1436,6 +1722,9 @@
       <c r="A15" t="s">
         <v>0</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
@@ -1444,6 +1733,9 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
@@ -1452,6 +1744,9 @@
       <c r="A17" t="s">
         <v>0</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="C17" t="s">
         <v>2</v>
       </c>
@@ -1460,6 +1755,9 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
@@ -1468,6 +1766,9 @@
       <c r="A19" t="s">
         <v>0</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
@@ -1476,6 +1777,9 @@
       <c r="A20" t="s">
         <v>0</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
@@ -1484,6 +1788,9 @@
       <c r="A21" t="s">
         <v>0</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
@@ -1492,6 +1799,9 @@
       <c r="A22" t="s">
         <v>0</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -1500,6 +1810,9 @@
       <c r="A23" t="s">
         <v>0</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
@@ -1508,6 +1821,9 @@
       <c r="A24" t="s">
         <v>0</v>
       </c>
+      <c r="B24" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
@@ -1516,6 +1832,9 @@
       <c r="A25" t="s">
         <v>0</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
@@ -1524,6 +1843,9 @@
       <c r="A26" t="s">
         <v>0</v>
       </c>
+      <c r="B26" s="1" t="s">
+        <v>325</v>
+      </c>
       <c r="C26" t="s">
         <v>2</v>
       </c>
@@ -1532,6 +1854,9 @@
       <c r="A27" t="s">
         <v>0</v>
       </c>
+      <c r="B27" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
@@ -1540,6 +1865,9 @@
       <c r="A28" t="s">
         <v>0</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
@@ -1548,6 +1876,9 @@
       <c r="A29" t="s">
         <v>0</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="C29" t="s">
         <v>2</v>
       </c>
@@ -1556,6 +1887,9 @@
       <c r="A30" t="s">
         <v>0</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
@@ -1564,6 +1898,9 @@
       <c r="A31" t="s">
         <v>0</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
@@ -1572,6 +1909,9 @@
       <c r="A32" t="s">
         <v>0</v>
       </c>
+      <c r="B32" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
@@ -1580,6 +1920,9 @@
       <c r="A33" t="s">
         <v>0</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
@@ -1588,6 +1931,9 @@
       <c r="A34" t="s">
         <v>0</v>
       </c>
+      <c r="B34" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="C34" t="s">
         <v>2</v>
       </c>
@@ -1596,6 +1942,9 @@
       <c r="A35" t="s">
         <v>0</v>
       </c>
+      <c r="B35" s="1" t="s">
+        <v>334</v>
+      </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
@@ -1604,6 +1953,9 @@
       <c r="A36" t="s">
         <v>0</v>
       </c>
+      <c r="B36" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
@@ -1612,6 +1964,9 @@
       <c r="A37" t="s">
         <v>0</v>
       </c>
+      <c r="B37" s="1" t="s">
+        <v>336</v>
+      </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
@@ -1620,6 +1975,9 @@
       <c r="A38" t="s">
         <v>0</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>337</v>
+      </c>
       <c r="C38" t="s">
         <v>2</v>
       </c>
@@ -1628,6 +1986,9 @@
       <c r="A39" t="s">
         <v>0</v>
       </c>
+      <c r="B39" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
@@ -1636,6 +1997,9 @@
       <c r="A40" t="s">
         <v>0</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>339</v>
+      </c>
       <c r="C40" t="s">
         <v>2</v>
       </c>
@@ -1644,6 +2008,9 @@
       <c r="A41" t="s">
         <v>0</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
@@ -1652,6 +2019,9 @@
       <c r="A42" t="s">
         <v>0</v>
       </c>
+      <c r="B42" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
@@ -1660,6 +2030,9 @@
       <c r="A43" t="s">
         <v>0</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
@@ -1668,6 +2041,9 @@
       <c r="A44" t="s">
         <v>0</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
@@ -1676,6 +2052,9 @@
       <c r="A45" t="s">
         <v>0</v>
       </c>
+      <c r="B45" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
@@ -1684,6 +2063,9 @@
       <c r="A46" t="s">
         <v>0</v>
       </c>
+      <c r="B46" s="1" t="s">
+        <v>345</v>
+      </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
@@ -1692,6 +2074,9 @@
       <c r="A47" t="s">
         <v>0</v>
       </c>
+      <c r="B47" s="1" t="s">
+        <v>346</v>
+      </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
@@ -1700,6 +2085,9 @@
       <c r="A48" t="s">
         <v>0</v>
       </c>
+      <c r="B48" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
@@ -1708,6 +2096,9 @@
       <c r="A49" t="s">
         <v>0</v>
       </c>
+      <c r="B49" s="1" t="s">
+        <v>348</v>
+      </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
@@ -1716,6 +2107,9 @@
       <c r="A50" t="s">
         <v>0</v>
       </c>
+      <c r="B50" s="1" t="s">
+        <v>349</v>
+      </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
@@ -1724,6 +2118,9 @@
       <c r="A51" t="s">
         <v>0</v>
       </c>
+      <c r="B51" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
@@ -1732,6 +2129,9 @@
       <c r="A52" t="s">
         <v>0</v>
       </c>
+      <c r="B52" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
@@ -1740,6 +2140,9 @@
       <c r="A53" t="s">
         <v>0</v>
       </c>
+      <c r="B53" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
@@ -1748,6 +2151,9 @@
       <c r="A54" t="s">
         <v>0</v>
       </c>
+      <c r="B54" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="C54" t="s">
         <v>2</v>
       </c>
@@ -1756,6 +2162,9 @@
       <c r="A55" t="s">
         <v>0</v>
       </c>
+      <c r="B55" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
@@ -1764,6 +2173,9 @@
       <c r="A56" t="s">
         <v>0</v>
       </c>
+      <c r="B56" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
@@ -1772,6 +2184,9 @@
       <c r="A57" t="s">
         <v>0</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
@@ -1780,6 +2195,9 @@
       <c r="A58" t="s">
         <v>0</v>
       </c>
+      <c r="B58" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
@@ -1788,6 +2206,9 @@
       <c r="A59" t="s">
         <v>0</v>
       </c>
+      <c r="B59" s="1" t="s">
+        <v>358</v>
+      </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
@@ -1796,6 +2217,9 @@
       <c r="A60" t="s">
         <v>0</v>
       </c>
+      <c r="B60" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
@@ -1804,6 +2228,9 @@
       <c r="A61" t="s">
         <v>0</v>
       </c>
+      <c r="B61" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
@@ -1812,6 +2239,9 @@
       <c r="A62" t="s">
         <v>0</v>
       </c>
+      <c r="B62" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
@@ -1820,6 +2250,9 @@
       <c r="A63" t="s">
         <v>0</v>
       </c>
+      <c r="B63" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
@@ -1828,6 +2261,9 @@
       <c r="A64" t="s">
         <v>0</v>
       </c>
+      <c r="B64" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="C64" t="s">
         <v>2</v>
       </c>
@@ -1836,6 +2272,9 @@
       <c r="A65" t="s">
         <v>0</v>
       </c>
+      <c r="B65" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="C65" t="s">
         <v>2</v>
       </c>
@@ -1844,6 +2283,9 @@
       <c r="A66" t="s">
         <v>0</v>
       </c>
+      <c r="B66" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
@@ -1852,6 +2294,7 @@
       <c r="A67" t="s">
         <v>0</v>
       </c>
+      <c r="B67" s="2"/>
       <c r="C67" t="s">
         <v>2</v>
       </c>
@@ -1860,6 +2303,9 @@
       <c r="A68" t="s">
         <v>0</v>
       </c>
+      <c r="B68" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
@@ -1868,6 +2314,9 @@
       <c r="A69" t="s">
         <v>0</v>
       </c>
+      <c r="B69" s="1" t="s">
+        <v>365</v>
+      </c>
       <c r="C69" t="s">
         <v>2</v>
       </c>
@@ -1876,6 +2325,9 @@
       <c r="A70" t="s">
         <v>0</v>
       </c>
+      <c r="B70" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="C70" t="s">
         <v>2</v>
       </c>
@@ -1884,6 +2336,9 @@
       <c r="A71" t="s">
         <v>0</v>
       </c>
+      <c r="B71" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
@@ -1892,6 +2347,9 @@
       <c r="A72" t="s">
         <v>0</v>
       </c>
+      <c r="B72" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
@@ -1900,6 +2358,9 @@
       <c r="A73" t="s">
         <v>0</v>
       </c>
+      <c r="B73" s="1" t="s">
+        <v>369</v>
+      </c>
       <c r="C73" t="s">
         <v>2</v>
       </c>
@@ -1908,6 +2369,9 @@
       <c r="A74" t="s">
         <v>0</v>
       </c>
+      <c r="B74" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="C74" t="s">
         <v>2</v>
       </c>
@@ -1916,6 +2380,9 @@
       <c r="A75" t="s">
         <v>0</v>
       </c>
+      <c r="B75" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="C75" t="s">
         <v>2</v>
       </c>
@@ -1924,6 +2391,9 @@
       <c r="A76" t="s">
         <v>0</v>
       </c>
+      <c r="B76" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="C76" t="s">
         <v>2</v>
       </c>
@@ -1932,6 +2402,9 @@
       <c r="A77" t="s">
         <v>0</v>
       </c>
+      <c r="B77" s="1" t="s">
+        <v>373</v>
+      </c>
       <c r="C77" t="s">
         <v>2</v>
       </c>
@@ -1940,6 +2413,9 @@
       <c r="A78" t="s">
         <v>0</v>
       </c>
+      <c r="B78" s="1" t="s">
+        <v>374</v>
+      </c>
       <c r="C78" t="s">
         <v>2</v>
       </c>
@@ -1948,6 +2424,9 @@
       <c r="A79" t="s">
         <v>0</v>
       </c>
+      <c r="B79" s="1" t="s">
+        <v>375</v>
+      </c>
       <c r="C79" t="s">
         <v>2</v>
       </c>
@@ -1956,6 +2435,9 @@
       <c r="A80" t="s">
         <v>0</v>
       </c>
+      <c r="B80" s="1" t="s">
+        <v>376</v>
+      </c>
       <c r="C80" t="s">
         <v>2</v>
       </c>
@@ -1964,6 +2446,9 @@
       <c r="A81" t="s">
         <v>0</v>
       </c>
+      <c r="B81" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="C81" t="s">
         <v>2</v>
       </c>
@@ -1972,6 +2457,9 @@
       <c r="A82" t="s">
         <v>0</v>
       </c>
+      <c r="B82" s="1" t="s">
+        <v>378</v>
+      </c>
       <c r="C82" t="s">
         <v>2</v>
       </c>
@@ -1980,6 +2468,9 @@
       <c r="A83" t="s">
         <v>0</v>
       </c>
+      <c r="B83" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="C83" t="s">
         <v>2</v>
       </c>
@@ -1988,6 +2479,9 @@
       <c r="A84" t="s">
         <v>0</v>
       </c>
+      <c r="B84" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="C84" t="s">
         <v>2</v>
       </c>
@@ -1996,6 +2490,9 @@
       <c r="A85" t="s">
         <v>0</v>
       </c>
+      <c r="B85" s="1" t="s">
+        <v>381</v>
+      </c>
       <c r="C85" t="s">
         <v>2</v>
       </c>
@@ -2004,6 +2501,9 @@
       <c r="A86" t="s">
         <v>0</v>
       </c>
+      <c r="B86" s="1" t="s">
+        <v>382</v>
+      </c>
       <c r="C86" t="s">
         <v>2</v>
       </c>
@@ -2012,6 +2512,9 @@
       <c r="A87" t="s">
         <v>0</v>
       </c>
+      <c r="B87" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="C87" t="s">
         <v>2</v>
       </c>
@@ -3641,6 +4144,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B66:B67"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3654,6 +4160,2374 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>0</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>0</v>
+      </c>
+      <c r="C108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>0</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>0</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>0</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>0</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>0</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>0</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>0</v>
+      </c>
+      <c r="C130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>0</v>
+      </c>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>0</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>0</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>0</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>0</v>
+      </c>
+      <c r="C138" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>0</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>0</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>0</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>0</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>0</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>0</v>
+      </c>
+      <c r="C150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>0</v>
+      </c>
+      <c r="C156" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>0</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>0</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>0</v>
+      </c>
+      <c r="C163" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>0</v>
+      </c>
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>0</v>
+      </c>
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>0</v>
+      </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>0</v>
+      </c>
+      <c r="C174" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
+        <v>0</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
+        <v>0</v>
+      </c>
+      <c r="C176" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>0</v>
+      </c>
+      <c r="C178" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>0</v>
+      </c>
+      <c r="C179" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
+        <v>0</v>
+      </c>
+      <c r="C180" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>0</v>
+      </c>
+      <c r="C181" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
+        <v>0</v>
+      </c>
+      <c r="C182" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>0</v>
+      </c>
+      <c r="C186" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>0</v>
+      </c>
+      <c r="C187" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="s">
+        <v>0</v>
+      </c>
+      <c r="C191" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C192" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
+        <v>0</v>
+      </c>
+      <c r="C193" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" t="s">
+        <v>0</v>
+      </c>
+      <c r="C194" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" t="s">
+        <v>0</v>
+      </c>
+      <c r="C195" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" t="s">
+        <v>0</v>
+      </c>
+      <c r="C196" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
+        <v>0</v>
+      </c>
+      <c r="C197" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
+        <v>0</v>
+      </c>
+      <c r="C198" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>0</v>
+      </c>
+      <c r="C199" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
+        <v>0</v>
+      </c>
+      <c r="C200" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>0</v>
+      </c>
+      <c r="C201" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" t="s">
+        <v>0</v>
+      </c>
+      <c r="C202" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>0</v>
+      </c>
+      <c r="C203" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
+        <v>0</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" t="s">
+        <v>0</v>
+      </c>
+      <c r="C205" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
+        <v>0</v>
+      </c>
+      <c r="C206" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" t="s">
+        <v>0</v>
+      </c>
+      <c r="C207" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" t="s">
+        <v>0</v>
+      </c>
+      <c r="C208" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" t="s">
+        <v>0</v>
+      </c>
+      <c r="C209" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" t="s">
+        <v>0</v>
+      </c>
+      <c r="C210" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" t="s">
+        <v>0</v>
+      </c>
+      <c r="C211" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" t="s">
+        <v>0</v>
+      </c>
+      <c r="C212" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>0</v>
+      </c>
+      <c r="C213" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
+        <v>0</v>
+      </c>
+      <c r="C214" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" t="s">
+        <v>0</v>
+      </c>
+      <c r="C215" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
+        <v>0</v>
+      </c>
+      <c r="C216" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
+        <v>0</v>
+      </c>
+      <c r="C217" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
+        <v>0</v>
+      </c>
+      <c r="C218" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>0</v>
+      </c>
+      <c r="C219" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C220" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>0</v>
+      </c>
+      <c r="C221" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" t="s">
+        <v>0</v>
+      </c>
+      <c r="C222" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
+        <v>0</v>
+      </c>
+      <c r="C223" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" t="s">
+        <v>0</v>
+      </c>
+      <c r="C224" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" t="s">
+        <v>0</v>
+      </c>
+      <c r="C225" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" t="s">
+        <v>0</v>
+      </c>
+      <c r="C226" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" t="s">
+        <v>0</v>
+      </c>
+      <c r="C227" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" t="s">
+        <v>0</v>
+      </c>
+      <c r="C229" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" t="s">
+        <v>0</v>
+      </c>
+      <c r="C230" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" t="s">
+        <v>0</v>
+      </c>
+      <c r="C231" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" t="s">
+        <v>0</v>
+      </c>
+      <c r="C232" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" t="s">
+        <v>0</v>
+      </c>
+      <c r="C233" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" t="s">
+        <v>0</v>
+      </c>
+      <c r="C234" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" t="s">
+        <v>0</v>
+      </c>
+      <c r="C235" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" t="s">
+        <v>0</v>
+      </c>
+      <c r="C236" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C237" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" t="s">
+        <v>0</v>
+      </c>
+      <c r="C238" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" t="s">
+        <v>0</v>
+      </c>
+      <c r="C239" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" t="s">
+        <v>0</v>
+      </c>
+      <c r="C240" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" t="s">
+        <v>0</v>
+      </c>
+      <c r="C241" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" t="s">
+        <v>0</v>
+      </c>
+      <c r="C242" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" t="s">
+        <v>0</v>
+      </c>
+      <c r="C243" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" t="s">
+        <v>0</v>
+      </c>
+      <c r="C244" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" t="s">
+        <v>0</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" t="s">
+        <v>0</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" t="s">
+        <v>0</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" t="s">
+        <v>0</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" t="s">
+        <v>0</v>
+      </c>
+      <c r="C250" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" t="s">
+        <v>0</v>
+      </c>
+      <c r="C251" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
+        <v>0</v>
+      </c>
+      <c r="C252" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" t="s">
+        <v>0</v>
+      </c>
+      <c r="C253" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
+        <v>0</v>
+      </c>
+      <c r="C254" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
+        <v>0</v>
+      </c>
+      <c r="C255" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" t="s">
+        <v>0</v>
+      </c>
+      <c r="C256" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" t="s">
+        <v>0</v>
+      </c>
+      <c r="C257" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" t="s">
+        <v>0</v>
+      </c>
+      <c r="C258" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" t="s">
+        <v>0</v>
+      </c>
+      <c r="C259" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" t="s">
+        <v>0</v>
+      </c>
+      <c r="C260" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" t="s">
+        <v>0</v>
+      </c>
+      <c r="C261" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" t="s">
+        <v>0</v>
+      </c>
+      <c r="C262" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" t="s">
+        <v>0</v>
+      </c>
+      <c r="C263" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" t="s">
+        <v>0</v>
+      </c>
+      <c r="C264" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" t="s">
+        <v>0</v>
+      </c>
+      <c r="C265" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" t="s">
+        <v>0</v>
+      </c>
+      <c r="C266" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
+        <v>0</v>
+      </c>
+      <c r="C267" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>0</v>
+      </c>
+      <c r="C268" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" t="s">
+        <v>0</v>
+      </c>
+      <c r="C269" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>0</v>
+      </c>
+      <c r="C270" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>0</v>
+      </c>
+      <c r="C271" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
+        <v>0</v>
+      </c>
+      <c r="C272" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>0</v>
+      </c>
+      <c r="C273" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>0</v>
+      </c>
+      <c r="C274" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>0</v>
+      </c>
+      <c r="C275" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>0</v>
+      </c>
+      <c r="C276" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
+        <v>0</v>
+      </c>
+      <c r="C277" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C278" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
+        <v>0</v>
+      </c>
+      <c r="C279" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>0</v>
+      </c>
+      <c r="C280" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
+        <v>0</v>
+      </c>
+      <c r="C281" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C282" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" t="s">
+        <v>0</v>
+      </c>
+      <c r="C283" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" t="s">
+        <v>0</v>
+      </c>
+      <c r="C284" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" t="s">
+        <v>0</v>
+      </c>
+      <c r="C285" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" t="s">
+        <v>0</v>
+      </c>
+      <c r="C286" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>0</v>
+      </c>
+      <c r="C287" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>0</v>
+      </c>
+      <c r="C288" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" t="s">
+        <v>0</v>
+      </c>
+      <c r="C289" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
+        <v>0</v>
+      </c>
+      <c r="C290" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C290"/>
+  <sheetViews>
     <sheetView showRuler="0" topLeftCell="A266" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
lots of writing; also, scaled tree down; cmd line option for tree
now you can call treegui like this: ./treeGUI "nice iced ink"
and it will make the tree for that phrase
</commit_message>
<xml_diff>
--- a/OronymsPushbacksTemplate.xlsx
+++ b/OronymsPushbacksTemplate.xlsx
@@ -11,7 +11,7 @@
     <sheet name="emptyOurEmailOronymsPushback" sheetId="2" r:id="rId2"/>
     <sheet name="anicecoldhourOronymsPushback.cs" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="448">
   <si>
     <t>orthoPhrases.push_back(</t>
   </si>
@@ -1016,9 +1016,6 @@
     <t>on ice coal dour</t>
   </si>
   <si>
-    <t>an i scold hour</t>
-  </si>
-  <si>
     <t>an iced cold hour</t>
   </si>
   <si>
@@ -1028,9 +1025,6 @@
     <t>in icecube daver</t>
   </si>
   <si>
-    <t>an ice cold bowl</t>
-  </si>
-  <si>
     <t>i saw tower</t>
   </si>
   <si>
@@ -1094,18 +1088,6 @@
     <t>in unschooled hour</t>
   </si>
   <si>
-    <t>in the eyeschool tower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in the ice cold hour </t>
-  </si>
-  <si>
-    <t>in ice called our</t>
-  </si>
-  <si>
-    <t>in the ice cold hour</t>
-  </si>
-  <si>
     <t>in ice coal dour</t>
   </si>
   <si>
@@ -1173,13 +1155,223 @@
   </si>
   <si>
     <t>on iced cold hour</t>
+  </si>
+  <si>
+    <t>an ice cold shower</t>
+  </si>
+  <si>
+    <t>on ice cold our</t>
+  </si>
+  <si>
+    <t>and i scold hour</t>
+  </si>
+  <si>
+    <t>a nice fold hour</t>
+  </si>
+  <si>
+    <t>Then ices co the where</t>
+  </si>
+  <si>
+    <t>enoise cothawer</t>
+  </si>
+  <si>
+    <t>and i scored the hour</t>
+  </si>
+  <si>
+    <t>a nice cold shower</t>
+  </si>
+  <si>
+    <t>an ice cold ower</t>
+  </si>
+  <si>
+    <t>a nice called hour</t>
+  </si>
+  <si>
+    <t>an ice cold bauer</t>
+  </si>
+  <si>
+    <t>The nice cold hour</t>
+  </si>
+  <si>
+    <t>a nice cold dollar</t>
+  </si>
+  <si>
+    <t>an ice cold grave</t>
+  </si>
+  <si>
+    <t>then ice go their were</t>
+  </si>
+  <si>
+    <t>he nice on the hour</t>
+  </si>
+  <si>
+    <t>a nine scold hour</t>
+  </si>
+  <si>
+    <t>on ice cold dour</t>
+  </si>
+  <si>
+    <t>in eye spole dower</t>
+  </si>
+  <si>
+    <t>a nine spole dower</t>
+  </si>
+  <si>
+    <t>a nigh scold hour</t>
+  </si>
+  <si>
+    <t>an nice cold our</t>
+  </si>
+  <si>
+    <t>hey nice hold hour</t>
+  </si>
+  <si>
+    <t>on ice co dover</t>
+  </si>
+  <si>
+    <t>ei nice cold hour</t>
+  </si>
+  <si>
+    <t>an ice ocld hour</t>
+  </si>
+  <si>
+    <t>ej nice cold ohur</t>
+  </si>
+  <si>
+    <t>an ice hold hour</t>
+  </si>
+  <si>
+    <t>ej nice cold hout</t>
+  </si>
+  <si>
+    <t>nice cold hour</t>
+  </si>
+  <si>
+    <t>a nice code hour</t>
+  </si>
+  <si>
+    <t>in ice cove diver</t>
+  </si>
+  <si>
+    <t>In ice cove daver</t>
+  </si>
+  <si>
+    <t>in nice code over</t>
+  </si>
+  <si>
+    <t>in nice code our</t>
+  </si>
+  <si>
+    <t>in ice gold hour</t>
+  </si>
+  <si>
+    <t>on eyes cold over</t>
+  </si>
+  <si>
+    <t>in eyes cold over</t>
+  </si>
+  <si>
+    <t>an I scold hour</t>
+  </si>
+  <si>
+    <t>a nice could hour</t>
+  </si>
+  <si>
+    <t>an ice cole dower</t>
+  </si>
+  <si>
+    <t>a nice cold dower</t>
+  </si>
+  <si>
+    <t>and i scored over</t>
+  </si>
+  <si>
+    <t>hey nine scold hour</t>
+  </si>
+  <si>
+    <t>the nice gold hour</t>
+  </si>
+  <si>
+    <t>A nice cold bowl</t>
+  </si>
+  <si>
+    <t>A nice cob bower</t>
+  </si>
+  <si>
+    <t>On ice core bower</t>
+  </si>
+  <si>
+    <t>An ice cold bowl</t>
+  </si>
+  <si>
+    <t>An ice bore bower</t>
+  </si>
+  <si>
+    <t>A nice pod our</t>
+  </si>
+  <si>
+    <t>An ice co bowel</t>
+  </si>
+  <si>
+    <t>An ice cob our</t>
+  </si>
+  <si>
+    <t>A nice cobour.</t>
+  </si>
+  <si>
+    <t>A nice cob our</t>
+  </si>
+  <si>
+    <t>in i scold hour</t>
+  </si>
+  <si>
+    <t>and nice cold hour</t>
+  </si>
+  <si>
+    <t>a nice cow is there</t>
+  </si>
+  <si>
+    <t>on eyes go there</t>
+  </si>
+  <si>
+    <t>an eyes co thou</t>
+  </si>
+  <si>
+    <t>an eyes close over</t>
+  </si>
+  <si>
+    <t>on ice call dour</t>
+  </si>
+  <si>
+    <t>a nice gold dour</t>
+  </si>
+  <si>
+    <t>hen eyes oh dawad</t>
+  </si>
+  <si>
+    <t>hen ice oh dawad</t>
+  </si>
+  <si>
+    <t>hen eyes oh gawd</t>
+  </si>
+  <si>
+    <t>an ice gold dower</t>
+  </si>
+  <si>
+    <t>a nice gold dower</t>
+  </si>
+  <si>
+    <t>orthoPhrases.push_back( "</t>
+  </si>
+  <si>
+    <t>" );</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1190,6 +1382,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1212,20 +1420,109 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -1554,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C290"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1566,1453 +1863,1641 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>301</v>
+        <v>337</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>302</v>
+        <v>446</v>
+      </c>
+      <c r="B3" t="s">
+        <v>300</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>303</v>
+        <v>446</v>
+      </c>
+      <c r="B4" t="s">
+        <v>366</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>304</v>
+        <v>365</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>306</v>
+        <v>446</v>
+      </c>
+      <c r="B7" t="s">
+        <v>307</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>308</v>
+        <v>446</v>
+      </c>
+      <c r="B9" t="s">
+        <v>321</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>310</v>
+        <v>378</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>446</v>
+      </c>
+      <c r="B12" t="s">
+        <v>332</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>312</v>
+        <v>446</v>
+      </c>
+      <c r="B13" t="s">
+        <v>316</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>313</v>
+        <v>446</v>
+      </c>
+      <c r="B14" t="s">
+        <v>308</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>314</v>
+        <v>446</v>
+      </c>
+      <c r="B15" t="s">
+        <v>345</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>315</v>
+        <v>446</v>
+      </c>
+      <c r="B16" t="s">
+        <v>335</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>316</v>
+        <v>446</v>
+      </c>
+      <c r="B17" t="s">
+        <v>314</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>317</v>
+        <v>446</v>
+      </c>
+      <c r="B18" t="s">
+        <v>320</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>318</v>
+        <v>446</v>
+      </c>
+      <c r="B19" t="s">
+        <v>317</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>319</v>
+        <v>446</v>
+      </c>
+      <c r="B20" t="s">
+        <v>310</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>320</v>
+        <v>446</v>
+      </c>
+      <c r="B21" t="s">
+        <v>354</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>321</v>
+        <v>379</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>323</v>
+        <v>380</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>324</v>
+        <v>381</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>326</v>
+        <v>446</v>
+      </c>
+      <c r="B27" t="s">
+        <v>367</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>327</v>
+        <v>382</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>328</v>
+        <v>383</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>329</v>
+        <v>384</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>330</v>
+        <v>446</v>
+      </c>
+      <c r="B31" t="s">
+        <v>315</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>331</v>
+        <v>446</v>
+      </c>
+      <c r="B32" t="s">
+        <v>357</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>332</v>
+        <v>446</v>
+      </c>
+      <c r="B33" t="s">
+        <v>341</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>333</v>
+        <v>446</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>385</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>334</v>
+        <v>386</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>335</v>
+        <v>387</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>337</v>
+        <v>388</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>339</v>
+        <v>389</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>340</v>
+        <v>390</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>341</v>
+        <v>391</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>342</v>
+        <v>446</v>
+      </c>
+      <c r="B43" t="s">
+        <v>319</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>343</v>
+        <v>392</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>345</v>
+        <v>393</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>346</v>
+        <v>394</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>347</v>
+        <v>303</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>348</v>
+        <v>395</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>349</v>
+        <v>396</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>350</v>
+        <v>397</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>351</v>
+        <v>446</v>
+      </c>
+      <c r="B52" t="s">
+        <v>329</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>352</v>
+        <v>446</v>
+      </c>
+      <c r="B53" t="s">
+        <v>362</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>353</v>
+        <v>446</v>
+      </c>
+      <c r="B54" t="s">
+        <v>372</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>355</v>
+        <v>398</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>356</v>
+        <v>399</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>357</v>
+        <v>400</v>
       </c>
       <c r="C58" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>358</v>
+        <v>401</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>359</v>
+        <v>402</v>
       </c>
       <c r="C60" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>360</v>
+        <v>403</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>361</v>
+        <v>404</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>362</v>
+        <v>446</v>
+      </c>
+      <c r="B63" t="s">
+        <v>353</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>363</v>
+        <v>405</v>
       </c>
       <c r="C64" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>134</v>
+        <v>406</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>302</v>
+        <v>446</v>
+      </c>
+      <c r="B66" t="s">
+        <v>301</v>
       </c>
       <c r="C66" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="2"/>
+        <v>446</v>
+      </c>
+      <c r="B67" t="s">
+        <v>364</v>
+      </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>364</v>
+        <v>446</v>
+      </c>
+      <c r="B68" t="s">
+        <v>369</v>
       </c>
       <c r="C68" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>365</v>
+        <v>446</v>
+      </c>
+      <c r="B69" t="s">
+        <v>356</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>366</v>
+        <v>407</v>
       </c>
       <c r="C70" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>367</v>
+        <v>446</v>
+      </c>
+      <c r="B71" t="s">
+        <v>322</v>
       </c>
       <c r="C71" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>368</v>
+        <v>446</v>
+      </c>
+      <c r="B72" t="s">
+        <v>338</v>
       </c>
       <c r="C72" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>369</v>
+        <v>446</v>
+      </c>
+      <c r="B73" t="s">
+        <v>331</v>
       </c>
       <c r="C73" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="C74" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>371</v>
+        <v>408</v>
       </c>
       <c r="C75" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="C76" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>373</v>
+        <v>446</v>
+      </c>
+      <c r="B77" t="s">
+        <v>343</v>
       </c>
       <c r="C77" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>374</v>
+        <v>409</v>
       </c>
       <c r="C78" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>375</v>
+        <v>446</v>
+      </c>
+      <c r="B79" t="s">
+        <v>333</v>
       </c>
       <c r="C79" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="C80" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>377</v>
+        <v>446</v>
+      </c>
+      <c r="B81" t="s">
+        <v>351</v>
       </c>
       <c r="C81" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>378</v>
+        <v>411</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>379</v>
+        <v>412</v>
       </c>
       <c r="C83" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="C84" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>381</v>
+        <v>414</v>
       </c>
       <c r="C85" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>382</v>
+        <v>415</v>
       </c>
       <c r="C86" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>383</v>
+        <v>361</v>
       </c>
       <c r="C87" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="C88" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B89" t="s">
+        <v>339</v>
       </c>
       <c r="C89" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B90" t="s">
+        <v>375</v>
       </c>
       <c r="C90" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B92" t="s">
+        <v>368</v>
       </c>
       <c r="C92" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B93" t="s">
+        <v>134</v>
       </c>
       <c r="C93" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B94" t="s">
+        <v>344</v>
       </c>
       <c r="C94" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>417</v>
       </c>
       <c r="C95" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B96" t="s">
+        <v>328</v>
       </c>
       <c r="C96" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B97" t="s">
+        <v>330</v>
       </c>
       <c r="C97" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>360</v>
       </c>
       <c r="C98" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>418</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B100" t="s">
+        <v>304</v>
       </c>
       <c r="C100" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>419</v>
       </c>
       <c r="C101" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>420</v>
       </c>
       <c r="C102" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B103" t="s">
+        <v>305</v>
       </c>
       <c r="C103" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B104" t="s">
+        <v>370</v>
       </c>
       <c r="C104" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B105" t="s">
+        <v>374</v>
       </c>
       <c r="C105" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B106" t="s">
+        <v>358</v>
       </c>
       <c r="C106" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B107" t="s">
+        <v>371</v>
       </c>
       <c r="C107" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B108" t="s">
+        <v>363</v>
       </c>
       <c r="C108" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B109" t="s">
+        <v>342</v>
       </c>
       <c r="C109" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B110" t="s">
+        <v>306</v>
       </c>
       <c r="C110" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B111" t="s">
+        <v>373</v>
       </c>
       <c r="C111" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>421</v>
       </c>
       <c r="C112" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B113" t="s">
+        <v>352</v>
       </c>
       <c r="C113" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="C114" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B115" t="s">
+        <v>311</v>
       </c>
       <c r="C115" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>302</v>
       </c>
       <c r="C116" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B117" t="s">
+        <v>325</v>
       </c>
       <c r="C117" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B118" t="s">
+        <v>312</v>
       </c>
       <c r="C118" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B119" t="s">
+        <v>313</v>
       </c>
       <c r="C119" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="C120" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>423</v>
       </c>
       <c r="C121" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>424</v>
       </c>
       <c r="C122" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="C123" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>346</v>
       </c>
       <c r="C124" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>426</v>
       </c>
       <c r="C125" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>427</v>
       </c>
       <c r="C126" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>428</v>
       </c>
       <c r="C127" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>429</v>
       </c>
       <c r="C128" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="C129" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>431</v>
       </c>
       <c r="C130" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="C131" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="C132" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="C133" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="C134" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B135" t="s">
+        <v>376</v>
       </c>
       <c r="C135" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B136" t="s">
+        <v>326</v>
       </c>
       <c r="C136" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="C137" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="C138" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="C139" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="C140" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>439</v>
       </c>
       <c r="C141" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>440</v>
       </c>
       <c r="C142" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="C143" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="C144" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="C145" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B146" t="s">
+        <v>377</v>
       </c>
       <c r="C146" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>444</v>
       </c>
       <c r="C147" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>445</v>
       </c>
       <c r="C148" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>0</v>
+        <v>446</v>
+      </c>
+      <c r="B149" t="s">
+        <v>334</v>
       </c>
       <c r="C149" t="s">
-        <v>2</v>
+        <v>447</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -4144,10 +4629,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B66:B67"/>
-  </mergeCells>
+  <conditionalFormatting sqref="B2:B149">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="an ice cold hour">
+      <formula>NOT(ISERROR(SEARCH("an ice cold hour",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B149">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="gold">
+      <formula>NOT(ISERROR(SEARCH("gold",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="a nice cold hour">
+      <formula>NOT(ISERROR(SEARCH("a nice cold hour",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Ran testWordBreakdown for all actual HIT transcriptions
Now, just got to merge my freq vals in Unique_HIT_transcriptions_with_freqVals.csv
with the TranscriptionHits_forMinitab spreadsheet.

I also may want to slightly tweak my wordBreakdown freq calculator to
do something weird when it doesn't find a word in a phrase.

Like explode.
</commit_message>
<xml_diff>
--- a/OronymsPushbacksTemplate.xlsx
+++ b/OronymsPushbacksTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="1900" yWindow="1280" windowWidth="25360" windowHeight="15140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ActualAnswersOronymsPushback" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2218" uniqueCount="481">
   <si>
     <t>orthoPhrases.push_back(</t>
   </si>
@@ -947,9 +947,6 @@
     <t>a nice old hour</t>
   </si>
   <si>
-    <t>a nice hold hour</t>
-  </si>
-  <si>
     <t>a nice gold hour</t>
   </si>
   <si>
@@ -1049,15 +1046,9 @@
     <t>a nice cool hour</t>
   </si>
   <si>
-    <t xml:space="preserve">can i score the hour  </t>
-  </si>
-  <si>
     <t>in ice co daver</t>
   </si>
   <si>
-    <t>an icecold hour</t>
-  </si>
-  <si>
     <t>an ice cold dollar</t>
   </si>
   <si>
@@ -1169,9 +1160,6 @@
     <t>a nice fold hour</t>
   </si>
   <si>
-    <t>Then ices co the where</t>
-  </si>
-  <si>
     <t>enoise cothawer</t>
   </si>
   <si>
@@ -1190,9 +1178,6 @@
     <t>an ice cold bauer</t>
   </si>
   <si>
-    <t>The nice cold hour</t>
-  </si>
-  <si>
     <t>a nice cold dollar</t>
   </si>
   <si>
@@ -1232,9 +1217,6 @@
     <t>ei nice cold hour</t>
   </si>
   <si>
-    <t>an ice ocld hour</t>
-  </si>
-  <si>
     <t>ej nice cold ohur</t>
   </si>
   <si>
@@ -1250,12 +1232,6 @@
     <t>a nice code hour</t>
   </si>
   <si>
-    <t>in ice cove diver</t>
-  </si>
-  <si>
-    <t>In ice cove daver</t>
-  </si>
-  <si>
     <t>in nice code over</t>
   </si>
   <si>
@@ -1271,9 +1247,6 @@
     <t>in eyes cold over</t>
   </si>
   <si>
-    <t>an I scold hour</t>
-  </si>
-  <si>
     <t>a nice could hour</t>
   </si>
   <si>
@@ -1289,39 +1262,6 @@
     <t>hey nine scold hour</t>
   </si>
   <si>
-    <t>the nice gold hour</t>
-  </si>
-  <si>
-    <t>A nice cold bowl</t>
-  </si>
-  <si>
-    <t>A nice cob bower</t>
-  </si>
-  <si>
-    <t>On ice core bower</t>
-  </si>
-  <si>
-    <t>An ice cold bowl</t>
-  </si>
-  <si>
-    <t>An ice bore bower</t>
-  </si>
-  <si>
-    <t>A nice pod our</t>
-  </si>
-  <si>
-    <t>An ice co bowel</t>
-  </si>
-  <si>
-    <t>An ice cob our</t>
-  </si>
-  <si>
-    <t>A nice cobour.</t>
-  </si>
-  <si>
-    <t>A nice cob our</t>
-  </si>
-  <si>
     <t>in i scold hour</t>
   </si>
   <si>
@@ -1365,6 +1305,165 @@
   </si>
   <si>
     <t>" );</t>
+  </si>
+  <si>
+    <t>Answer.answer</t>
+  </si>
+  <si>
+    <t>can i score the hour</t>
+  </si>
+  <si>
+    <t>ni screwdriver</t>
+  </si>
+  <si>
+    <t>can i spoke hour</t>
+  </si>
+  <si>
+    <t>a nice screwdriver</t>
+  </si>
+  <si>
+    <t>in high school hour</t>
+  </si>
+  <si>
+    <t>an ice go the our</t>
+  </si>
+  <si>
+    <t>a nice screw driver</t>
+  </si>
+  <si>
+    <t>we nice old hour</t>
+  </si>
+  <si>
+    <t>the nice cold hour</t>
+  </si>
+  <si>
+    <t>an ice hold power</t>
+  </si>
+  <si>
+    <t>hey nice screwdriver</t>
+  </si>
+  <si>
+    <t>a nice school bower</t>
+  </si>
+  <si>
+    <t>make noice whole the hour</t>
+  </si>
+  <si>
+    <t>hey nice go there where</t>
+  </si>
+  <si>
+    <t>n i screwdriver</t>
+  </si>
+  <si>
+    <t>an i scold hour</t>
+  </si>
+  <si>
+    <t>in ice called our</t>
+  </si>
+  <si>
+    <t>in the ice cold hour</t>
+  </si>
+  <si>
+    <t>in the eyeschool tower</t>
+  </si>
+  <si>
+    <t>in a ice cool hour</t>
+  </si>
+  <si>
+    <t>then ice go there  our</t>
+  </si>
+  <si>
+    <t>a nine skulled hour</t>
+  </si>
+  <si>
+    <t>a nice scold dower</t>
+  </si>
+  <si>
+    <t>in ice old hour</t>
+  </si>
+  <si>
+    <t>a nice for the hour</t>
+  </si>
+  <si>
+    <t>hey nice go the our</t>
+  </si>
+  <si>
+    <t>an i scold dour</t>
+  </si>
+  <si>
+    <t>an eye scold our</t>
+  </si>
+  <si>
+    <t>an i screwdriver</t>
+  </si>
+  <si>
+    <t>an ice cold bowl</t>
+  </si>
+  <si>
+    <t>in ice cold dour</t>
+  </si>
+  <si>
+    <t>an ice cool bower</t>
+  </si>
+  <si>
+    <t>then ice hole power</t>
+  </si>
+  <si>
+    <t>an i screw driver</t>
+  </si>
+  <si>
+    <t>an ice-cold hour</t>
+  </si>
+  <si>
+    <t>in ice-cold hour</t>
+  </si>
+  <si>
+    <t>an iced cold dower</t>
+  </si>
+  <si>
+    <t>on i screwdriver</t>
+  </si>
+  <si>
+    <t>an eyes hold power</t>
+  </si>
+  <si>
+    <t>a nice cool dower</t>
+  </si>
+  <si>
+    <t>a nice cold hout</t>
+  </si>
+  <si>
+    <t>a nice go the our</t>
+  </si>
+  <si>
+    <t>a nice cob bower</t>
+  </si>
+  <si>
+    <t>a nice cob our</t>
+  </si>
+  <si>
+    <t>a nice cobour</t>
+  </si>
+  <si>
+    <t>a nice cold bowl</t>
+  </si>
+  <si>
+    <t>a nice pod our</t>
+  </si>
+  <si>
+    <t>an ice bore bower</t>
+  </si>
+  <si>
+    <t>an ice cob our</t>
+  </si>
+  <si>
+    <t>in ice go tower</t>
+  </si>
+  <si>
+    <t>on ice core bower</t>
+  </si>
+  <si>
+    <t>then ices co the where</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1519,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1434,34 +1533,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1479,36 +1615,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1852,7 +1958,7 @@
   <dimension ref="A1:C290"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1863,1889 +1969,1982 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>426</v>
+      </c>
+      <c r="B1" t="s">
+        <v>428</v>
       </c>
       <c r="C1" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>337</v>
+        <v>356</v>
       </c>
       <c r="C2" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>446</v>
-      </c>
-      <c r="B3" t="s">
-        <v>300</v>
+        <v>426</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="C3" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>446</v>
-      </c>
-      <c r="B4" t="s">
-        <v>366</v>
+        <v>426</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>383</v>
       </c>
       <c r="C4" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>365</v>
+        <v>306</v>
       </c>
       <c r="C5" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C6" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>446</v>
-      </c>
-      <c r="B7" t="s">
-        <v>307</v>
+        <v>426</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>471</v>
       </c>
       <c r="C7" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>309</v>
+        <v>472</v>
       </c>
       <c r="C8" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>446</v>
-      </c>
-      <c r="B9" t="s">
-        <v>321</v>
+        <v>426</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>473</v>
       </c>
       <c r="C9" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>324</v>
+        <v>402</v>
       </c>
       <c r="C10" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>378</v>
+        <v>474</v>
       </c>
       <c r="C11" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>446</v>
-      </c>
-      <c r="B12" t="s">
-        <v>332</v>
+        <v>426</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>385</v>
       </c>
       <c r="C12" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>446</v>
-      </c>
-      <c r="B13" t="s">
-        <v>316</v>
+        <v>426</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="C13" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>446</v>
-      </c>
-      <c r="B14" t="s">
-        <v>308</v>
+        <v>426</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>410</v>
       </c>
       <c r="C14" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>446</v>
-      </c>
-      <c r="B15" t="s">
-        <v>345</v>
+        <v>426</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="C15" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>446</v>
-      </c>
-      <c r="B16" t="s">
-        <v>335</v>
+        <v>426</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>469</v>
       </c>
       <c r="C16" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>446</v>
-      </c>
-      <c r="B17" t="s">
-        <v>314</v>
+        <v>426</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="C17" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>446</v>
-      </c>
-      <c r="B18" t="s">
-        <v>320</v>
+        <v>426</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>381</v>
       </c>
       <c r="C18" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>446</v>
-      </c>
-      <c r="B19" t="s">
-        <v>317</v>
+        <v>426</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="C19" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>446</v>
-      </c>
-      <c r="B20" t="s">
-        <v>310</v>
+        <v>426</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="C20" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>446</v>
-      </c>
-      <c r="B21" t="s">
+        <v>426</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>354</v>
       </c>
       <c r="C21" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>379</v>
+        <v>468</v>
       </c>
       <c r="C22" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="C23" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>380</v>
+        <v>408</v>
       </c>
       <c r="C24" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>381</v>
+        <v>415</v>
       </c>
       <c r="C25" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>318</v>
+        <v>378</v>
       </c>
       <c r="C26" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>446</v>
-      </c>
-      <c r="B27" t="s">
-        <v>367</v>
+        <v>426</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="C27" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>382</v>
+        <v>470</v>
       </c>
       <c r="C28" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>383</v>
+        <v>318</v>
       </c>
       <c r="C29" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>384</v>
+        <v>314</v>
       </c>
       <c r="C30" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>446</v>
-      </c>
-      <c r="B31" t="s">
-        <v>315</v>
+        <v>426</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>420</v>
       </c>
       <c r="C31" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>446</v>
-      </c>
-      <c r="B32" t="s">
-        <v>357</v>
+        <v>426</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>425</v>
       </c>
       <c r="C32" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>446</v>
-      </c>
-      <c r="B33" t="s">
-        <v>341</v>
+        <v>426</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="C33" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>446</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>385</v>
+        <v>426</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="C34" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>386</v>
+        <v>307</v>
       </c>
       <c r="C35" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>387</v>
+        <v>475</v>
       </c>
       <c r="C36" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>340</v>
+        <v>370</v>
       </c>
       <c r="C37" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>388</v>
+        <v>440</v>
       </c>
       <c r="C38" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>350</v>
+        <v>451</v>
       </c>
       <c r="C39" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>389</v>
+        <v>310</v>
       </c>
       <c r="C40" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>390</v>
+        <v>309</v>
       </c>
       <c r="C41" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>391</v>
+        <v>435</v>
       </c>
       <c r="C42" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>446</v>
-      </c>
-      <c r="B43" t="s">
-        <v>319</v>
+        <v>426</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="C43" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>392</v>
+        <v>316</v>
       </c>
       <c r="C44" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="C45" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>393</v>
+        <v>346</v>
       </c>
       <c r="C46" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C47" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C48" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C49" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>396</v>
+        <v>450</v>
       </c>
       <c r="C50" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C51" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>446</v>
-      </c>
-      <c r="B52" t="s">
-        <v>329</v>
+        <v>426</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="C52" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>446</v>
-      </c>
-      <c r="B53" t="s">
-        <v>362</v>
+        <v>426</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="C53" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>446</v>
-      </c>
-      <c r="B54" t="s">
-        <v>372</v>
+        <v>426</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="C54" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>323</v>
+        <v>366</v>
       </c>
       <c r="C55" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>398</v>
+        <v>324</v>
       </c>
       <c r="C56" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>399</v>
+        <v>322</v>
       </c>
       <c r="C57" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>400</v>
+        <v>456</v>
       </c>
       <c r="C58" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="C59" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>402</v>
+        <v>417</v>
       </c>
       <c r="C60" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>403</v>
+        <v>325</v>
       </c>
       <c r="C61" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>404</v>
+        <v>467</v>
       </c>
       <c r="C62" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>446</v>
-      </c>
-      <c r="B63" t="s">
-        <v>353</v>
+        <v>426</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>455</v>
       </c>
       <c r="C63" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>405</v>
+        <v>444</v>
       </c>
       <c r="C64" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>406</v>
+        <v>462</v>
       </c>
       <c r="C65" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>446</v>
-      </c>
-      <c r="B66" t="s">
-        <v>301</v>
+        <v>426</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>457</v>
       </c>
       <c r="C66" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>446</v>
-      </c>
-      <c r="B67" t="s">
-        <v>364</v>
+        <v>426</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>476</v>
       </c>
       <c r="C67" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>446</v>
-      </c>
-      <c r="B68" t="s">
-        <v>369</v>
+        <v>426</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="C68" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>446</v>
-      </c>
-      <c r="B69" t="s">
-        <v>356</v>
+        <v>426</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="C69" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>407</v>
+        <v>335</v>
       </c>
       <c r="C70" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>446</v>
-      </c>
-      <c r="B71" t="s">
-        <v>322</v>
+        <v>426</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>477</v>
       </c>
       <c r="C71" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>446</v>
-      </c>
-      <c r="B72" t="s">
-        <v>338</v>
+        <v>426</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="C72" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>446</v>
-      </c>
-      <c r="B73" t="s">
-        <v>331</v>
+        <v>426</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="C73" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>349</v>
+        <v>458</v>
       </c>
       <c r="C74" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>408</v>
+        <v>342</v>
       </c>
       <c r="C75" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C76" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>446</v>
-      </c>
-      <c r="B77" t="s">
-        <v>343</v>
+        <v>426</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="C77" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="C78" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>446</v>
-      </c>
-      <c r="B79" t="s">
-        <v>333</v>
+        <v>426</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="C79" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>410</v>
+        <v>319</v>
       </c>
       <c r="C80" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>446</v>
-      </c>
-      <c r="B81" t="s">
-        <v>351</v>
+        <v>426</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>382</v>
       </c>
       <c r="C81" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>411</v>
+        <v>375</v>
       </c>
       <c r="C82" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>412</v>
+        <v>355</v>
       </c>
       <c r="C83" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C84" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>414</v>
+        <v>460</v>
       </c>
       <c r="C85" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>415</v>
+        <v>343</v>
       </c>
       <c r="C86" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="C87" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C88" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>446</v>
-      </c>
-      <c r="B89" t="s">
-        <v>339</v>
+        <v>426</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="C89" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>446</v>
-      </c>
-      <c r="B90" t="s">
-        <v>375</v>
+        <v>426</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>424</v>
       </c>
       <c r="C90" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>416</v>
+        <v>320</v>
       </c>
       <c r="C91" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>446</v>
-      </c>
-      <c r="B92" t="s">
-        <v>368</v>
+        <v>426</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>399</v>
       </c>
       <c r="C92" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>446</v>
-      </c>
-      <c r="B93" t="s">
-        <v>134</v>
+        <v>426</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>438</v>
       </c>
       <c r="C93" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>446</v>
-      </c>
-      <c r="B94" t="s">
-        <v>344</v>
+        <v>426</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="C94" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>417</v>
+        <v>321</v>
       </c>
       <c r="C95" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>446</v>
-      </c>
-      <c r="B96" t="s">
-        <v>328</v>
+        <v>426</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>463</v>
       </c>
       <c r="C96" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>446</v>
-      </c>
-      <c r="B97" t="s">
-        <v>330</v>
+        <v>426</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>465</v>
       </c>
       <c r="C97" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="C98" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>418</v>
+        <v>357</v>
       </c>
       <c r="C99" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>446</v>
-      </c>
-      <c r="B100" t="s">
-        <v>304</v>
+        <v>426</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>394</v>
       </c>
       <c r="C100" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>419</v>
+        <v>327</v>
       </c>
       <c r="C101" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>420</v>
+        <v>377</v>
       </c>
       <c r="C102" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>446</v>
-      </c>
-      <c r="B103" t="s">
-        <v>305</v>
+        <v>426</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="C103" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>446</v>
-      </c>
-      <c r="B104" t="s">
-        <v>370</v>
+        <v>426</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>411</v>
       </c>
       <c r="C104" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>446</v>
-      </c>
-      <c r="B105" t="s">
-        <v>374</v>
+        <v>426</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>380</v>
       </c>
       <c r="C105" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>446</v>
-      </c>
-      <c r="B106" t="s">
-        <v>358</v>
+        <v>426</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="C106" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>446</v>
-      </c>
-      <c r="B107" t="s">
-        <v>371</v>
+        <v>426</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>414</v>
       </c>
       <c r="C107" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>446</v>
-      </c>
-      <c r="B108" t="s">
-        <v>363</v>
+        <v>426</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>429</v>
       </c>
       <c r="C108" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>446</v>
-      </c>
-      <c r="B109" t="s">
-        <v>342</v>
+        <v>426</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>431</v>
       </c>
       <c r="C109" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>446</v>
-      </c>
-      <c r="B110" t="s">
-        <v>306</v>
+        <v>426</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>397</v>
       </c>
       <c r="C110" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>446</v>
-      </c>
-      <c r="B111" t="s">
-        <v>373</v>
+        <v>426</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>400</v>
       </c>
       <c r="C111" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="C112" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>446</v>
-      </c>
-      <c r="B113" t="s">
-        <v>352</v>
+        <v>426</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>379</v>
       </c>
       <c r="C113" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>446</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>422</v>
+        <v>426</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="C114" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>446</v>
-      </c>
-      <c r="B115" t="s">
-        <v>311</v>
+        <v>426</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>421</v>
       </c>
       <c r="C115" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>446</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>302</v>
+        <v>426</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>423</v>
       </c>
       <c r="C116" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>446</v>
-      </c>
-      <c r="B117" t="s">
-        <v>325</v>
+        <v>426</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>422</v>
       </c>
       <c r="C117" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>446</v>
-      </c>
-      <c r="B118" t="s">
-        <v>312</v>
+        <v>426</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>454</v>
       </c>
       <c r="C118" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>446</v>
-      </c>
-      <c r="B119" t="s">
-        <v>313</v>
+        <v>426</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>442</v>
       </c>
       <c r="C119" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>347</v>
+        <v>395</v>
       </c>
       <c r="C120" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>423</v>
+        <v>439</v>
       </c>
       <c r="C121" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="C122" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>425</v>
+        <v>333</v>
       </c>
       <c r="C123" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C124" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>426</v>
+        <v>448</v>
       </c>
       <c r="C125" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>446</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>391</v>
       </c>
       <c r="C126" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="C127" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C128" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="C129" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="C130" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>432</v>
+        <v>341</v>
       </c>
       <c r="C131" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C132" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>433</v>
+        <v>348</v>
       </c>
       <c r="C133" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>434</v>
+        <v>331</v>
       </c>
       <c r="C134" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>446</v>
-      </c>
-      <c r="B135" t="s">
-        <v>376</v>
+        <v>426</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="C135" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>446</v>
-      </c>
-      <c r="B136" t="s">
+        <v>426</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>326</v>
       </c>
       <c r="C136" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>435</v>
+        <v>353</v>
       </c>
       <c r="C137" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>436</v>
+        <v>478</v>
       </c>
       <c r="C138" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>437</v>
+        <v>405</v>
       </c>
       <c r="C139" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="C140" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>439</v>
+        <v>464</v>
       </c>
       <c r="C141" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>440</v>
+        <v>332</v>
       </c>
       <c r="C142" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>441</v>
+        <v>404</v>
       </c>
       <c r="C143" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>442</v>
+        <v>403</v>
       </c>
       <c r="C144" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>443</v>
+        <v>358</v>
       </c>
       <c r="C145" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>446</v>
-      </c>
-      <c r="B146" t="s">
-        <v>377</v>
+        <v>426</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>447</v>
       </c>
       <c r="C146" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
+        <v>426</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>444</v>
-      </c>
       <c r="C147" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>445</v>
+        <v>351</v>
       </c>
       <c r="C148" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>446</v>
-      </c>
-      <c r="B149" t="s">
-        <v>334</v>
+        <v>426</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>441</v>
       </c>
       <c r="C149" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="C150" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="C151" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="C152" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>371</v>
       </c>
       <c r="C153" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>369</v>
       </c>
       <c r="C154" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>406</v>
       </c>
       <c r="C155" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="C156" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>466</v>
       </c>
       <c r="C157" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>419</v>
       </c>
       <c r="C158" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>361</v>
       </c>
       <c r="C159" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="C160" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="C161" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="C162" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>372</v>
       </c>
       <c r="C163" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>364</v>
       </c>
       <c r="C164" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="C165" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>363</v>
       </c>
       <c r="C166" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>362</v>
       </c>
       <c r="C167" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>376</v>
       </c>
       <c r="C168" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>367</v>
       </c>
       <c r="C169" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>479</v>
       </c>
       <c r="C170" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>368</v>
       </c>
       <c r="C171" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>374</v>
       </c>
       <c r="C172" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>365</v>
       </c>
       <c r="C173" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>360</v>
       </c>
       <c r="C174" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="C175" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>387</v>
       </c>
       <c r="C176" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>449</v>
       </c>
       <c r="C177" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="C178" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="C179" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>0</v>
+        <v>426</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="C180" t="s">
-        <v>2</v>
+        <v>427</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -4629,19 +4828,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B149">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="an ice cold hour">
-      <formula>NOT(ISERROR(SEARCH("an ice cold hour",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B149">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="gold">
-      <formula>NOT(ISERROR(SEARCH("gold",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="a nice cold hour">
-      <formula>NOT(ISERROR(SEARCH("a nice cold hour",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>